<commit_message>
bulk upload and analysis done
</commit_message>
<xml_diff>
--- a/uploads/reviews.xlsx
+++ b/uploads/reviews.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28526"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28623"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\zish0\OneDrive\Desktop\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4CC66080-CEFF-457E-A651-85A506070A67}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FECFF683-11B4-4DC3-A22E-9B48191F072F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11310" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
   <si>
     <t>review</t>
   </si>
@@ -33,10 +33,19 @@
     <t>I love this product</t>
   </si>
   <si>
-    <t>this is terrible.</t>
-  </si>
-  <si>
-    <t>It's okay.</t>
+    <t>this is not good product</t>
+  </si>
+  <si>
+    <t xml:space="preserve">nice product but costly </t>
+  </si>
+  <si>
+    <t xml:space="preserve">product is far away from my budget but it is very helpful </t>
+  </si>
+  <si>
+    <t xml:space="preserve">your overall service is very good </t>
+  </si>
+  <si>
+    <t xml:space="preserve">I am very satisfied with this product </t>
   </si>
 </sst>
 </file>
@@ -354,13 +363,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:A4"/>
+  <dimension ref="A1:A7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A4" sqref="A4"/>
+      <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="21.5703125" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
@@ -382,6 +394,21 @@
         <v>3</v>
       </c>
     </row>
+    <row r="5" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="6" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="7" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>6</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>